<commit_message>
minor fix for text after grouping
</commit_message>
<xml_diff>
--- a/samples/xlsx/TestTemplateBasicIEmumerableFillGroup.xlsx
+++ b/samples/xlsx/TestTemplateBasicIEmumerableFillGroup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\Eynar_Haji\MiniExcel\samples\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7C9A2E24-4F6D-48F6-BAE7-E62F98BAD189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7029C7FF-28E2-4B28-BC03-8EFD53F3040C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B1F1315B-82EC-4C2D-BCFD-4048ED09EB0D}"/>
+    <workbookView xWindow="45" yWindow="1485" windowWidth="21555" windowHeight="11415" xr2:uid="{B1F1315B-82EC-4C2D-BCFD-4048ED09EB0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>@header{{employees.name}}</t>
+  </si>
+  <si>
+    <t>Text after</t>
   </si>
 </sst>
 </file>
@@ -143,10 +146,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -463,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A400F1-56C5-4363-8B40-8D5ADCB945EF}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,10 +493,10 @@
       <c r="B2" s="2"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="5"/>
+      <c r="B3" s="6"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -506,6 +509,21 @@
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix unit tests and docs
</commit_message>
<xml_diff>
--- a/samples/xlsx/TestTemplateBasicIEmumerableFillGroup.xlsx
+++ b/samples/xlsx/TestTemplateBasicIEmumerableFillGroup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\Eynar_Haji\MiniExcel\samples\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7029C7FF-28E2-4B28-BC03-8EFD53F3040C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B702A8D4-CA1D-4D45-AFB9-36FCAF798E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="1485" windowWidth="21555" windowHeight="11415" xr2:uid="{B1F1315B-82EC-4C2D-BCFD-4048ED09EB0D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B1F1315B-82EC-4C2D-BCFD-4048ED09EB0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -140,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -151,6 +151,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,7 +472,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A7" sqref="A7:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,18 +520,17 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
+      <c r="A8" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add support for merge vertical cells automatically (#467)
* add support for grouped cells

* fix for rows after endgroup

* minor fix for text after grouping

* fix unit tests

* fix unit tests and docs

* minor fix

* Add support to vertical merge cells
</commit_message>
<xml_diff>
--- a/samples/xlsx/TestTemplateBasicIEmumerableFillGroup.xlsx
+++ b/samples/xlsx/TestTemplateBasicIEmumerableFillGroup.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Developer\Eynar_Haji\MiniExcel\samples\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7029C7FF-28E2-4B28-BC03-8EFD53F3040C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B702A8D4-CA1D-4D45-AFB9-36FCAF798E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="1485" windowWidth="21555" windowHeight="11415" xr2:uid="{B1F1315B-82EC-4C2D-BCFD-4048ED09EB0D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{B1F1315B-82EC-4C2D-BCFD-4048ED09EB0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -140,7 +140,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -151,6 +151,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -469,7 +472,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A7" sqref="A7:A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,18 +520,17 @@
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
+      <c r="A8" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A7:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>